<commit_message>
dropped _ from entries
</commit_message>
<xml_diff>
--- a/forager-cochlear/data/lexical_data/animals/corrections.xlsx
+++ b/forager-cochlear/data/lexical_data/animals/corrections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bowdoin-my.sharepoint.com/personal/c_hambric_bowdoin_edu/Documents/Documents/cochlear-full/forager-cochlear/data/lexical_data/animals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\forager-cochlear\data\lexical_data\animals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{325F64F7-F093-8845-9505-EFEC9273BACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D48BAF4A-FDFA-4AE0-9B6D-E3D9F183E064}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6FEB9D-16A1-4C98-A6EE-74B39B8AA43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F57B2306-9FF8-F542-99A6-1BB4FDAC2DD8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F57B2306-9FF8-F542-99A6-1BB4FDAC2DD8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,9 +167,6 @@
     <t>raccoon</t>
   </si>
   <si>
-    <t>saber_tooth_cat</t>
-  </si>
-  <si>
     <t>lion</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
     <t>stegosaurus</t>
   </si>
   <si>
-    <t>t_rex</t>
-  </si>
-  <si>
     <t>tarantula</t>
   </si>
   <si>
@@ -314,10 +308,16 @@
     <t>shark</t>
   </si>
   <si>
-    <t>ring_tailed</t>
-  </si>
-  <si>
     <t>prairie</t>
+  </si>
+  <si>
+    <t>sabertoothcat</t>
+  </si>
+  <si>
+    <t>trex</t>
+  </si>
+  <si>
+    <t>ringtailed</t>
   </si>
 </sst>
 </file>
@@ -383,10 +383,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -708,21 +704,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48052F7A-DB63-5D4A-9278-ACFD2E5A2B47}">
   <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -730,7 +726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -738,15 +734,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -754,7 +750,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -762,23 +758,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -786,7 +782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -794,23 +790,23 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -818,15 +814,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -834,7 +830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -842,7 +838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
@@ -850,7 +846,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -858,7 +854,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -866,7 +862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -874,7 +870,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -882,7 +878,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -890,7 +886,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>28</v>
       </c>
@@ -898,15 +894,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>30</v>
       </c>
@@ -914,7 +910,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
@@ -922,7 +918,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>34</v>
       </c>
@@ -930,15 +926,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
@@ -946,15 +942,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>38</v>
       </c>
@@ -962,15 +958,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>40</v>
       </c>
@@ -978,7 +974,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>42</v>
       </c>
@@ -986,212 +982,212 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="B36" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
         <v>49</v>
       </c>
-      <c r="B38" t="s">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>51</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="B43" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>52</v>
+      </c>
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>54</v>
-      </c>
-      <c r="B44" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>56</v>
       </c>
       <c r="B46" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B47" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>75</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>77</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B51" t="s">
         <v>79</v>
       </c>
-      <c r="B50" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>80</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>82</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>84</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B55" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>86</v>
-      </c>
-      <c r="B54" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>87</v>
-      </c>
-      <c r="B55" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>88</v>
       </c>
       <c r="B56" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" t="s">
         <v>89</v>
       </c>
-      <c r="B57" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>90</v>
       </c>
-      <c r="B58" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>92</v>
-      </c>
-      <c r="B59" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>93</v>
-      </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>